<commit_message>
Fix date handling in test
</commit_message>
<xml_diff>
--- a/src/test/resources/complex.xlsx
+++ b/src/test/resources/complex.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Numdiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Accepted</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -66,13 +72,14 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="d&quot;. &quot;mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,13 +96,33 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,7 +134,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,12 +158,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,19 +184,84 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEFEFEF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -166,163 +270,217 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>43952</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="4" t="n">
         <v>43952.6549768519</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3.252</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="n">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <f aca="false">C2-D2</f>
         <v>96.748</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="G2" s="5" t="n">
+        <v>43613</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>43953</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="4" t="n">
         <v>43953.6549884259</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4.255</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="n">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <f aca="false">C3-D3</f>
         <v>96.745</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="G3" s="5" t="n">
+        <v>43647</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>43954</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="4" t="n">
         <v>43954.655</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5.222</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <f aca="false">C4-D4</f>
         <v>96.778</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="G4" s="5" t="n">
+        <v>43654</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>43955</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="4" t="n">
         <v>43955.6550115741</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>6.981</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="n">
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <f aca="false">C5-D5</f>
         <v>96.019</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="G5" s="5" t="n">
+        <v>43676</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>43956</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="4" t="n">
         <v>43956.6550231482</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>7.125</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="n">
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <f aca="false">C6-D6</f>
         <v>96.875</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="G6" s="5" t="n">
+        <v>43709</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>43957</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="4" t="n">
         <v>43957.6550347223</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>8.021</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="n">
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <f aca="false">C7-D7</f>
         <v>96.979</v>
       </c>
+      <c r="G7" s="5" t="n">
+        <v>43806</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>43806</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
make ods import behave similar to excel when importing percentages (i.e import it as a decimal e.g. 0.54 instead of 54%) improve test upgrade poi and slf4j
</commit_message>
<xml_diff>
--- a/src/test/resources/complex.xlsx
+++ b/src/test/resources/complex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Date Accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractions</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -78,11 +81,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="d&quot;. &quot;mmmm\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.00%"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -173,7 +177,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,6 +204,10 @@
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -280,217 +288,238 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="A2:D3 E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="J2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
         <v>43952</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="C3" s="4" t="n">
         <v>43952.6549768519</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="D3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>3.252</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <f aca="false">C2-D2</f>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <f aca="false">D3-E3</f>
         <v>96.748</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="H3" s="5" t="n">
         <v>43613</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="I3" s="6" t="n">
         <v>43613</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="J3" s="7" t="n">
+        <f aca="false">E3/D3</f>
+        <v>0.03252</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="n">
         <v>43953</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="C4" s="4" t="n">
         <v>43953.6549884259</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="D4" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E4" s="1" t="n">
         <v>4.255</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">C3-D3</f>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <f aca="false">D4-E4</f>
         <v>96.745</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="H4" s="5" t="n">
         <v>43647</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="I4" s="6" t="n">
         <v>43647</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="J4" s="7" t="n">
+        <f aca="false">E4/D4</f>
+        <v>0.0421287128712871</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3" t="n">
         <v>43954</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="C5" s="4" t="n">
         <v>43954.655</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="D5" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="E5" s="1" t="n">
         <v>5.222</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">C4-D4</f>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <f aca="false">D5-E5</f>
         <v>96.778</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="H5" s="5" t="n">
         <v>43654</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="I5" s="6" t="n">
         <v>43647</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="J5" s="7" t="n">
+        <f aca="false">E5/D5</f>
+        <v>0.0511960784313726</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3" t="n">
         <v>43955</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="C6" s="4" t="n">
         <v>43955.6550115741</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="D6" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="E6" s="1" t="n">
         <v>6.981</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">C5-D5</f>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">D6-E6</f>
         <v>96.019</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="H6" s="5" t="n">
         <v>43676</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="I6" s="6" t="n">
         <v>43676</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="J6" s="7" t="n">
+        <f aca="false">E6/D6</f>
+        <v>0.0677766990291262</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="n">
         <v>43956</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="C7" s="4" t="n">
         <v>43956.6550231482</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="D7" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="E7" s="1" t="n">
         <v>7.125</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">C6-D6</f>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <f aca="false">D7-E7</f>
         <v>96.875</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="H7" s="5" t="n">
         <v>43709</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="I7" s="6" t="n">
         <v>43709</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>43957</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>43957.6550347223</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>8.021</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">C7-D7</f>
-        <v>96.979</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>43806</v>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>43806</v>
+      <c r="J7" s="7" t="n">
+        <f aca="false">E7/D7</f>
+        <v>0.0685096153846154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1"/>
+      <c r="B8" s="3" t="n">
+        <v>43957</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>43957.6550347223</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>8.021</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <f aca="false">D8-E8</f>
+        <v>96.979</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>43806</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>43806</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <f aca="false">E8/D8</f>
+        <v>0.0763904761904762</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -510,15 +539,15 @@
   </sheetPr>
   <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2020</v>
@@ -526,7 +555,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">BEG</f>

</xml_diff>